<commit_message>
Updated with latest results. Had to do it on a machine with Excel on it as Numbers creates inflated xlsx files...
</commit_message>
<xml_diff>
--- a/19.xlsx
+++ b/19.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="101">
   <si>
     <t>Test all connections listed in the table below and record the values observed. Use the test points on the adapter board.</t>
   </si>
@@ -225,9 +225,6 @@
     <t>Final decision:</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>1) Do not connect the adapter. Turn HV on, read after 60 sec</t>
   </si>
   <si>
@@ -319,6 +316,15 @@
   </si>
   <si>
     <t>Corrected</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Brian / Frank</t>
   </si>
 </sst>
 </file>
@@ -428,8 +434,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="181">
+  <cellStyleXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -697,14 +707,14 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="181">
+  <cellStyles count="185">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -795,6 +805,8 @@
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -885,6 +897,8 @@
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1238,8 +1252,8 @@
   </sheetPr>
   <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1248,21 +1262,21 @@
     <col min="3" max="3" width="8.33203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="9"/>
-    <col min="6" max="6" width="11" style="5"/>
+    <col min="6" max="6" width="11.5" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.83203125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="26.25">
+    <row r="1" spans="1:15" ht="25">
       <c r="A1" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="18.75">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="18">
       <c r="A3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="31">
@@ -1272,13 +1286,13 @@
     <row r="4" spans="1:15">
       <c r="B4" s="27"/>
     </row>
-    <row r="5" spans="1:15" ht="18.75">
+    <row r="5" spans="1:15" ht="18">
       <c r="A5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="27"/>
       <c r="C5" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>47</v>
@@ -1286,17 +1300,17 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="27"/>
       <c r="C6" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="30">
         <v>79980109</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H6" s="26">
         <v>0.1</v>
@@ -1307,11 +1321,11 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="27"/>
       <c r="C7" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D7" s="30">
         <v>26</v>
@@ -1319,11 +1333,11 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="27"/>
       <c r="C8" s="29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="30">
         <v>1268080</v>
@@ -1333,7 +1347,7 @@
       <c r="B9" s="27"/>
       <c r="C9" s="20"/>
     </row>
-    <row r="11" spans="1:15" ht="18.75">
+    <row r="11" spans="1:15" ht="18">
       <c r="A11" s="1" t="s">
         <v>53</v>
       </c>
@@ -1431,10 +1445,12 @@
       <c r="J18" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="12"/>
+      <c r="K18" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L18" s="9" t="str">
         <f t="shared" ref="L18:L33" si="0">IF(AND(K18&lt;K$34,ISNUMBER(K18)),"ok","NOK")</f>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O18">
         <f t="shared" ref="O18:O51" si="1">IF(G18="NOK",1,0)</f>
@@ -1442,7 +1458,7 @@
       </c>
       <c r="P18">
         <f>IF(L18="NOK",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -1474,10 +1490,12 @@
       <c r="J19" t="s">
         <v>14</v>
       </c>
-      <c r="K19" s="12"/>
+      <c r="K19" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L19" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O19">
         <f t="shared" si="1"/>
@@ -1485,7 +1503,7 @@
       </c>
       <c r="P19">
         <f t="shared" ref="P19:P33" si="2">IF(L19="NOK",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1518,10 +1536,12 @@
       <c r="J20" t="s">
         <v>9</v>
       </c>
-      <c r="K20" s="12"/>
+      <c r="K20" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L20" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O20">
         <f t="shared" si="1"/>
@@ -1529,7 +1549,7 @@
       </c>
       <c r="P20">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1562,10 +1582,12 @@
       <c r="J21" t="s">
         <v>9</v>
       </c>
-      <c r="K21" s="12"/>
+      <c r="K21" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L21" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O21">
         <f t="shared" si="1"/>
@@ -1573,7 +1595,7 @@
       </c>
       <c r="P21">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1605,10 +1627,12 @@
       <c r="J22" t="s">
         <v>15</v>
       </c>
-      <c r="K22" s="12"/>
+      <c r="K22" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L22" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O22">
         <f t="shared" si="1"/>
@@ -1616,7 +1640,7 @@
       </c>
       <c r="P22">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1648,10 +1672,12 @@
       <c r="J23" t="s">
         <v>16</v>
       </c>
-      <c r="K23" s="12"/>
+      <c r="K23" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L23" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O23">
         <f t="shared" si="1"/>
@@ -1659,7 +1685,7 @@
       </c>
       <c r="P23">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -1691,10 +1717,12 @@
       <c r="J24" t="s">
         <v>17</v>
       </c>
-      <c r="K24" s="12"/>
+      <c r="K24" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L24" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O24">
         <f t="shared" si="1"/>
@@ -1702,7 +1730,7 @@
       </c>
       <c r="P24">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -1734,10 +1762,12 @@
       <c r="J25" t="s">
         <v>18</v>
       </c>
-      <c r="K25" s="12"/>
+      <c r="K25" s="12">
+        <v>0.8</v>
+      </c>
       <c r="L25" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O25">
         <f t="shared" si="1"/>
@@ -1745,7 +1775,7 @@
       </c>
       <c r="P25">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -1777,10 +1807,12 @@
       <c r="J26" t="s">
         <v>19</v>
       </c>
-      <c r="K26" s="12"/>
+      <c r="K26" s="12">
+        <v>0.8</v>
+      </c>
       <c r="L26" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O26">
         <f t="shared" si="1"/>
@@ -1788,7 +1820,7 @@
       </c>
       <c r="P26">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -1820,10 +1852,12 @@
       <c r="J27" t="s">
         <v>20</v>
       </c>
-      <c r="K27" s="12"/>
+      <c r="K27" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L27" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O27">
         <f t="shared" si="1"/>
@@ -1831,7 +1865,7 @@
       </c>
       <c r="P27">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -1863,10 +1897,12 @@
       <c r="J28" t="s">
         <v>21</v>
       </c>
-      <c r="K28" s="12"/>
+      <c r="K28" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L28" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O28">
         <f t="shared" si="1"/>
@@ -1874,7 +1910,7 @@
       </c>
       <c r="P28">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -1906,10 +1942,12 @@
       <c r="J29" t="s">
         <v>22</v>
       </c>
-      <c r="K29" s="12"/>
+      <c r="K29" s="12">
+        <v>0.6</v>
+      </c>
       <c r="L29" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O29">
         <f t="shared" si="1"/>
@@ -1917,7 +1955,7 @@
       </c>
       <c r="P29">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -1949,10 +1987,12 @@
       <c r="J30" t="s">
         <v>10</v>
       </c>
-      <c r="K30" s="12"/>
+      <c r="K30" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L30" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O30">
         <f t="shared" si="1"/>
@@ -1960,7 +2000,7 @@
       </c>
       <c r="P30">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -1992,10 +2032,12 @@
       <c r="J31" t="s">
         <v>10</v>
       </c>
-      <c r="K31" s="12"/>
+      <c r="K31" s="12">
+        <v>0.8</v>
+      </c>
       <c r="L31" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O31">
         <f t="shared" si="1"/>
@@ -2003,7 +2045,7 @@
       </c>
       <c r="P31">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -2036,10 +2078,12 @@
       <c r="J32" t="s">
         <v>11</v>
       </c>
-      <c r="K32" s="12"/>
+      <c r="K32" s="12">
+        <v>0.8</v>
+      </c>
       <c r="L32" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O32">
         <f t="shared" si="1"/>
@@ -2047,7 +2091,7 @@
       </c>
       <c r="P32">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -2079,10 +2123,12 @@
       <c r="J33" t="s">
         <v>12</v>
       </c>
-      <c r="K33" s="12"/>
+      <c r="K33" s="12">
+        <v>0.8</v>
+      </c>
       <c r="L33" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O33">
         <f t="shared" si="1"/>
@@ -2090,7 +2136,7 @@
       </c>
       <c r="P33">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -2182,12 +2228,12 @@
         <f>IF(ABS(F36-D36)&lt;=E36,"ok","NOK")</f>
         <v>ok</v>
       </c>
-      <c r="I36" s="35" t="s">
+      <c r="I36" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="J36" s="35"/>
-      <c r="K36" s="35"/>
-      <c r="L36" s="35"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="36"/>
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
       <c r="O36">
@@ -2327,10 +2373,12 @@
       <c r="J40" t="s">
         <v>8</v>
       </c>
-      <c r="K40" s="12"/>
+      <c r="K40" s="12">
+        <v>0.3</v>
+      </c>
       <c r="L40" s="9" t="str">
         <f t="shared" ref="L40:L47" si="5">IF(AND(K40&lt;K$48,ISNUMBER(K40)),"ok","NOK")</f>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O40">
         <f t="shared" si="1"/>
@@ -2338,7 +2386,7 @@
       </c>
       <c r="P40">
         <f t="shared" ref="P40:P47" si="6">IF(L40="NOK",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:16">
@@ -2371,10 +2419,12 @@
       <c r="J41" t="s">
         <v>8</v>
       </c>
-      <c r="K41" s="12"/>
+      <c r="K41" s="12">
+        <v>0.3</v>
+      </c>
       <c r="L41" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O41">
         <f t="shared" si="1"/>
@@ -2382,7 +2432,7 @@
       </c>
       <c r="P41">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:16">
@@ -2415,10 +2465,12 @@
       <c r="J42" t="s">
         <v>9</v>
       </c>
-      <c r="K42" s="12"/>
+      <c r="K42" s="12">
+        <v>0.3</v>
+      </c>
       <c r="L42" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O42">
         <f t="shared" si="1"/>
@@ -2426,7 +2478,7 @@
       </c>
       <c r="P42">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -2460,10 +2512,12 @@
       <c r="J43" t="s">
         <v>8</v>
       </c>
-      <c r="K43" s="12"/>
+      <c r="K43" s="12">
+        <v>0.3</v>
+      </c>
       <c r="L43" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O43">
         <f t="shared" si="1"/>
@@ -2471,7 +2525,7 @@
       </c>
       <c r="P43">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -2505,10 +2559,12 @@
       <c r="J44" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K44" s="12"/>
+      <c r="K44" s="12">
+        <v>0.3</v>
+      </c>
       <c r="L44" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O44">
         <f t="shared" si="1"/>
@@ -2516,7 +2572,7 @@
       </c>
       <c r="P44">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:16">
@@ -2537,7 +2593,7 @@
         <f>SQRT((39*0.05)^2+(91*0.05)^2+(39*0.05)^2)</f>
         <v>5.3204793017170928</v>
       </c>
-      <c r="F45" s="36">
+      <c r="F45" s="35">
         <v>168.9</v>
       </c>
       <c r="G45" s="5" t="str">
@@ -2550,10 +2606,12 @@
       <c r="J45" t="s">
         <v>10</v>
       </c>
-      <c r="K45" s="12"/>
+      <c r="K45" s="12">
+        <v>0.3</v>
+      </c>
       <c r="L45" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O45">
         <f t="shared" si="1"/>
@@ -2561,7 +2619,7 @@
       </c>
       <c r="P45">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:16">
@@ -2582,11 +2640,11 @@
         <v>5.1961524227066312E-2</v>
       </c>
       <c r="F46" s="13">
-        <v>29.85</v>
+        <v>30</v>
       </c>
       <c r="G46" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="I46">
         <v>8</v>
@@ -2594,18 +2652,20 @@
       <c r="J46" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K46" s="12"/>
+      <c r="K46" s="12">
+        <v>0.3</v>
+      </c>
       <c r="L46" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O46">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P46">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:16">
@@ -2637,10 +2697,12 @@
       <c r="J47" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K47" s="12"/>
+      <c r="K47" s="12">
+        <v>0.3</v>
+      </c>
       <c r="L47" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O47">
         <f t="shared" si="1"/>
@@ -2648,7 +2710,7 @@
       </c>
       <c r="P47">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:16">
@@ -2787,15 +2849,15 @@
       </c>
       <c r="B53" s="14" t="str">
         <f>IF(SUM(O18:O51,P18:P33,P40:P47)&gt;0,"FAIL","PASS")</f>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" ht="18.75">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="18">
       <c r="A55" s="1" t="s">
         <v>37</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
@@ -2812,12 +2874,12 @@
         <v>38</v>
       </c>
       <c r="I57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J57" s="14"/>
       <c r="K57" s="5"/>
       <c r="M57" s="30" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:15">
@@ -2828,31 +2890,33 @@
         <v>43</v>
       </c>
       <c r="I58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J58" s="14"/>
       <c r="K58" s="5"/>
       <c r="M58" s="30" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:15">
       <c r="I59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J59" s="14"/>
       <c r="K59" s="5"/>
       <c r="M59" s="30" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:15">
       <c r="A60" t="s">
         <v>39</v>
       </c>
-      <c r="B60" s="23"/>
-    </row>
-    <row r="62" spans="1:15" ht="18.75">
+      <c r="B60" s="23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="18">
       <c r="A62" s="1" t="s">
         <v>41</v>
       </c>
@@ -2865,7 +2929,7 @@
         <v>42</v>
       </c>
       <c r="I64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="65" spans="1:13">
@@ -2876,86 +2940,94 @@
         <v>44</v>
       </c>
       <c r="I65" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J65" s="24"/>
       <c r="K65" s="16"/>
     </row>
     <row r="66" spans="1:13">
       <c r="B66" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I66" t="s">
+        <v>85</v>
+      </c>
+      <c r="K66" s="32">
+        <v>98.8</v>
+      </c>
+      <c r="L66" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="K66" s="32"/>
-      <c r="L66" s="5" t="s">
+      <c r="M66" s="17" t="s">
         <v>87</v>
-      </c>
-      <c r="M66" s="17" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="67" spans="1:13">
       <c r="B67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I67" t="s">
-        <v>89</v>
-      </c>
-      <c r="K67" s="32"/>
+        <v>88</v>
+      </c>
+      <c r="K67" s="32">
+        <v>9.91</v>
+      </c>
       <c r="L67" s="5" t="s">
         <v>45</v>
       </c>
       <c r="M67" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="68" spans="1:13">
       <c r="B68" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="1:13">
       <c r="I69" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K69" s="33">
         <f>102000*K67*0.000001</f>
-        <v>0</v>
+        <v>1.0108200000000001</v>
       </c>
       <c r="L69" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:13">
       <c r="B70" t="s">
-        <v>71</v>
-      </c>
-      <c r="C70" s="24"/>
+        <v>70</v>
+      </c>
+      <c r="C70" s="24">
+        <v>1.7999999999999999E-2</v>
+      </c>
       <c r="D70" s="4" t="s">
         <v>45</v>
       </c>
       <c r="I70" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="71" spans="1:13">
       <c r="B71" t="s">
-        <v>72</v>
-      </c>
-      <c r="C71" s="24"/>
+        <v>71</v>
+      </c>
+      <c r="C71" s="24">
+        <v>1.9E-2</v>
+      </c>
       <c r="D71" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="72" spans="1:13">
       <c r="B72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C72" s="24">
         <f>C71-C70</f>
-        <v>0</v>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>45</v>
@@ -2970,14 +3042,14 @@
         <v>45</v>
       </c>
       <c r="I72" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K72" s="18">
         <f>K66+K69</f>
-        <v>0</v>
+        <v>99.810819999999993</v>
       </c>
       <c r="L72" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:13">
@@ -2996,31 +3068,35 @@
       </c>
       <c r="B75" s="14" t="str">
         <f>IF(AND(C72&lt;=F72,ABS(K72-100)&lt;0.5),"PASS","FAIL")</f>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
     </row>
     <row r="77" spans="1:13">
       <c r="B77" s="14"/>
     </row>
-    <row r="78" spans="1:13" ht="18.75">
+    <row r="78" spans="1:13" ht="18">
       <c r="A78" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B78" s="14"/>
       <c r="C78" s="22" t="str">
         <f>IF(AND(B53="PASS",B60="PASS",B75="PASS",M57="y",M58="y",M59="y"),"ACCEPTED","REJECTED")</f>
-        <v>REJECTED</v>
+        <v>ACCEPTED</v>
       </c>
     </row>
     <row r="80" spans="1:13">
       <c r="A80" t="s">
         <v>48</v>
       </c>
-      <c r="B80" s="26"/>
+      <c r="B80" s="26" t="s">
+        <v>100</v>
+      </c>
       <c r="E80" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F80" s="34"/>
+      <c r="F80" s="34">
+        <v>41908</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>